<commit_message>
Updated Sprint 2 Burndown Sheet
Added 3 more Acceptance Tests for Sprint 1 and 2
</commit_message>
<xml_diff>
--- a/Group24 - Sprint2 Burndown.xlsx
+++ b/Group24 - Sprint2 Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\New Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnol\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE8132E-C230-467E-B7DF-11768AAC5002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C82663-F6EE-4117-A896-650969774A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="28830" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Sprint Plan 2</t>
   </si>
@@ -273,6 +273,45 @@
   <si>
     <t>#50</t>
   </si>
+  <si>
+    <t>Acceptance Test (AT) 1.3: Task.10 Create Team</t>
+  </si>
+  <si>
+    <t>Issue Tracking
+This acceptance test is for #10
+User Acceptance FI
+Users fills in Create Team form
+If user leaves one of the data blank or both, then an error message will display prompting the fields as Required before submitting
+If user inputs a Team name that already exists, an error message will show and the team will not be created
+User submits the fields of Create Team
+User will see the newly created team on the list of Teams in "View Teams" tab</t>
+  </si>
+  <si>
+    <t>Acceptance Test (AT) 1.4: Task.12 (Instructor) Assign Student #12</t>
+  </si>
+  <si>
+    <t>Issue Tracking
+This acceptance test is for #12
+User Acceptance FI
+User clicks "Assign Member" button
+If user attempts to assign a member to a team with full capacity, an error message will display and member will not be assigned to that team
+User assigns the Member to a team
+System should display the newly assigned member to the team in the student list table</t>
+  </si>
+  <si>
+    <t>Acceptance Test (AT) 2.1: US.30</t>
+  </si>
+  <si>
+    <t>Issue Tracking
+This acceptance test is for user story #30
+User Acceptance FI
+User clicks "View Team"
+If user does not belong to a group, interface will display no members with group "None"
+If user is alone in the group, interface will display them as the only member and unable to assess themselves
+If user is part of a group with members other than themselves, interface will display all members with buttons next to each member for assessment except the logged in user
+User clicks "Assess Member"
+Upon clicking, peer review page is loaded for assessing the selected member</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m\-d\-yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -316,6 +355,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -343,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -384,6 +429,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:H1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1073,22 +1121,83 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.75">
-      <c r="B19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.75">
-      <c r="B20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.75">
-      <c r="B21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="H21" s="14"/>
+    <row r="19" spans="1:8" ht="185.25">
+      <c r="A19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="9">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10">
+        <v>45591</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="156.75">
+      <c r="A20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="9">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10">
+        <v>45591</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="199.5">
+      <c r="A21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="9">
+        <v>9</v>
+      </c>
+      <c r="D21" s="10">
+        <v>45591</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="12.75">
       <c r="B22" s="13"/>
@@ -5991,5 +6100,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>